<commit_message>
Predictions of week 2 added to the repo
</commit_message>
<xml_diff>
--- a/predictions/eltigre_competition.xlsx
+++ b/predictions/eltigre_competition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somidi\GitLab\ET_covid19_prediction_project\predictions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somidi\GitLab\ElTigre_Covid19_Prediction\predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3543BCE-D619-4F37-B624-43BFB508930A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4480D3F3-084D-46E0-999E-FEDA628B4FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25665" yWindow="-2145" windowWidth="22395" windowHeight="13170" activeTab="1" xr2:uid="{39BC2CFF-1192-4BC4-A950-9DBD52F813F4}"/>
+    <workbookView xWindow="-25620" yWindow="-825" windowWidth="19185" windowHeight="10200" activeTab="1" xr2:uid="{39BC2CFF-1192-4BC4-A950-9DBD52F813F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Alex</t>
   </si>
@@ -91,6 +91,27 @@
   </si>
   <si>
     <t>Dr. Brauwolf</t>
+  </si>
+  <si>
+    <t>Japon_death</t>
+  </si>
+  <si>
+    <t>Japon_total</t>
+  </si>
+  <si>
+    <t>Chile_total</t>
+  </si>
+  <si>
+    <t>Chile_death</t>
+  </si>
+  <si>
+    <t>Israel_total</t>
+  </si>
+  <si>
+    <t>Israel_death</t>
+  </si>
+  <si>
+    <t>Vasco</t>
   </si>
 </sst>
 </file>
@@ -648,7 +669,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F4:F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,42 +706,156 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>3900</v>
+      </c>
+      <c r="C2">
+        <v>4000</v>
+      </c>
+      <c r="D2">
+        <v>3800</v>
+      </c>
       <c r="E2" s="1"/>
+      <c r="F2">
+        <v>6000</v>
+      </c>
       <c r="H2" s="1">
         <v>43925</v>
       </c>
+      <c r="I2">
+        <v>4800</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>85</v>
+      </c>
+      <c r="D3">
+        <v>115</v>
+      </c>
       <c r="E3" s="1"/>
+      <c r="F3">
+        <v>200</v>
+      </c>
       <c r="H3" s="1">
         <v>43925</v>
       </c>
+      <c r="I3">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>7200</v>
+      </c>
+      <c r="C4">
+        <v>5000</v>
+      </c>
+      <c r="D4">
+        <v>7450</v>
+      </c>
       <c r="E4" s="1"/>
+      <c r="F4">
+        <v>7000</v>
+      </c>
       <c r="H4" s="1">
         <v>43925</v>
       </c>
+      <c r="I4">
+        <v>6400</v>
+      </c>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>108</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>84</v>
+      </c>
       <c r="E5" s="1"/>
+      <c r="F5">
+        <v>150</v>
+      </c>
       <c r="H5" s="1">
         <v>43925</v>
       </c>
+      <c r="I5">
+        <v>55</v>
+      </c>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>11100</v>
+      </c>
+      <c r="C6">
+        <v>11000</v>
+      </c>
+      <c r="D6">
+        <v>11250</v>
+      </c>
       <c r="E6" s="1"/>
+      <c r="F6">
+        <v>12000</v>
+      </c>
       <c r="H6" s="1">
         <v>43925</v>
       </c>
+      <c r="I6">
+        <v>11000</v>
+      </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>88</v>
+      </c>
+      <c r="C7">
+        <v>300</v>
+      </c>
+      <c r="D7">
+        <v>87</v>
+      </c>
       <c r="E7" s="1"/>
+      <c r="F7">
+        <v>400</v>
+      </c>
+      <c r="H7" s="1">
+        <v>43925</v>
+      </c>
+      <c r="I7">
+        <v>75</v>
+      </c>
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>